<commit_message>
Documentation finis et ajustement appellation document
</commit_message>
<xml_diff>
--- a/Documentation/Gestion De Projet.xlsx
+++ b/Documentation/Gestion De Projet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garri\Documents\TP_Web_Garrigues\ProjetWeb-Th-o-Hugo\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Desktop\ProjetWeb-Theo-Hugo\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A02916-358C-48FE-9567-5F9F374D32EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58835868-900B-4471-94F0-C3F3D0855F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>Tâches / Fonctions</t>
   </si>
@@ -51,16 +51,31 @@
     <t>ScrollSnap</t>
   </si>
   <si>
-    <t>Argentique</t>
-  </si>
-  <si>
-    <t>Numérique</t>
-  </si>
-  <si>
-    <t>Portrait</t>
-  </si>
-  <si>
     <t>Page d'accueil</t>
+  </si>
+  <si>
+    <t>Page voiture</t>
+  </si>
+  <si>
+    <t>Hugo</t>
+  </si>
+  <si>
+    <t>Italie</t>
+  </si>
+  <si>
+    <t>Allemagne</t>
+  </si>
+  <si>
+    <t>Japon</t>
+  </si>
+  <si>
+    <t>Css Histoire</t>
+  </si>
+  <si>
+    <t>Css caracteristiques</t>
+  </si>
+  <si>
+    <t>Html Voitures</t>
   </si>
 </sst>
 </file>
@@ -102,10 +117,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,21 +402,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -417,81 +433,173 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1">
+        <v>44935</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44939</v>
+      </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1">
+        <v>44935</v>
+      </c>
+      <c r="D3" s="1">
+        <v>44937</v>
+      </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1">
+        <v>44935</v>
+      </c>
+      <c r="D4" s="1">
+        <v>44936</v>
+      </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1">
+        <v>44936</v>
+      </c>
+      <c r="D5" s="1">
+        <v>44939</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1">
+        <v>44936</v>
+      </c>
+      <c r="D6" s="1">
+        <v>44939</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1">
+        <v>44936</v>
+      </c>
+      <c r="D7" s="1">
+        <v>44939</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1">
+        <v>44935</v>
+      </c>
+      <c r="D8" s="1">
+        <v>44940</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1">
+        <v>44937</v>
+      </c>
+      <c r="D9" s="1">
+        <v>44940</v>
+      </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1">
+        <v>44937</v>
+      </c>
+      <c r="D10" s="1">
+        <v>44940</v>
+      </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1">
+        <v>44937</v>
+      </c>
+      <c r="D11" s="1">
+        <v>44940</v>
+      </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1">
+        <v>44937</v>
+      </c>
+      <c r="D12" s="1">
+        <v>44940</v>
+      </c>
       <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>